<commit_message>
To be or not to be
</commit_message>
<xml_diff>
--- a/LR3/table_1_29.xlsx
+++ b/LR3/table_1_29.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9921BFA5-80FC-4959-81A8-A6AABEB3FA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43C4B7A3-5DAE-4E3C-8C2A-21D96C63809E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="924" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -510,6 +510,7 @@
     <col min="2" max="2" width="37.77734375" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
     <col min="8" max="8" width="19.5546875" customWidth="1"/>
     <col min="9" max="9" width="16.109375" customWidth="1"/>
   </cols>
@@ -606,6 +607,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
+        <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -635,6 +637,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
+        <f>I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="5">
@@ -648,6 +651,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
+        <f t="shared" ref="A5:A38" si="7">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -677,6 +681,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="4">
+        <f t="shared" ref="I5:I38" si="8">I4</f>
         <v>10</v>
       </c>
       <c r="J5" s="5">
@@ -690,6 +695,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -719,6 +725,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J6" s="5">
@@ -732,6 +739,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -761,6 +769,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J7" s="5">
@@ -774,6 +783,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -803,6 +813,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J8" s="5">
@@ -816,6 +827,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -845,6 +857,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J9" s="5">
@@ -858,6 +871,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -887,6 +901,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J10" s="5">
@@ -900,6 +915,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -929,6 +945,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J11" s="5">
@@ -942,6 +959,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -971,6 +989,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J12" s="5">
@@ -984,6 +1003,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1013,6 +1033,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J13" s="5">
@@ -1026,6 +1047,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1055,6 +1077,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J14" s="5">
@@ -1068,6 +1091,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1097,6 +1121,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J15" s="5">
@@ -1110,6 +1135,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1139,6 +1165,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J16" s="5">
@@ -1152,6 +1179,7 @@
     </row>
     <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1181,6 +1209,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J17" s="5">
@@ -1194,6 +1223,7 @@
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1223,6 +1253,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J18" s="5">
@@ -1236,6 +1267,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1265,6 +1297,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J19" s="5">
@@ -1278,6 +1311,7 @@
     </row>
     <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -1307,6 +1341,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J20" s="5">
@@ -1320,6 +1355,7 @@
     </row>
     <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1349,6 +1385,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J21" s="5">
@@ -1362,6 +1399,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1391,6 +1429,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J22" s="5">
@@ -1404,6 +1443,7 @@
     </row>
     <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
@@ -1433,6 +1473,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J23" s="5">
@@ -1446,6 +1487,7 @@
     </row>
     <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="B24" s="11" t="s">
@@ -1475,6 +1517,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J24" s="5">
@@ -1488,6 +1531,7 @@
     </row>
     <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
@@ -1517,6 +1561,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J25" s="5">
@@ -1530,6 +1575,7 @@
     </row>
     <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -1559,6 +1605,7 @@
         <v>15</v>
       </c>
       <c r="I26" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J26" s="5">
@@ -1572,6 +1619,7 @@
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -1601,6 +1649,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J27" s="5">
@@ -1614,6 +1663,7 @@
     </row>
     <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -1643,6 +1693,7 @@
         <v>17</v>
       </c>
       <c r="I28" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J28" s="5">
@@ -1656,6 +1707,7 @@
     </row>
     <row r="29" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -1685,6 +1737,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J29" s="5">
@@ -1698,6 +1751,7 @@
     </row>
     <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -1727,6 +1781,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J30" s="5">
@@ -1740,6 +1795,7 @@
     </row>
     <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
@@ -1769,6 +1825,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J31" s="5">
@@ -1782,6 +1839,7 @@
     </row>
     <row r="32" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
@@ -1811,6 +1869,7 @@
         <v>21</v>
       </c>
       <c r="I32" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J32" s="5">
@@ -1824,6 +1883,7 @@
     </row>
     <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
@@ -1853,6 +1913,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J33" s="5">
@@ -1866,6 +1927,7 @@
     </row>
     <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
@@ -1895,6 +1957,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J34" s="5">
@@ -1908,6 +1971,7 @@
     </row>
     <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -1918,7 +1982,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="5">
-        <f t="shared" ref="D35:D38" si="7">((29)*1.1)/2</f>
+        <f t="shared" ref="D35:D38" si="9">((29)*1.1)/2</f>
         <v>15.950000000000001</v>
       </c>
       <c r="E35" s="5">
@@ -1937,6 +2001,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J35" s="5">
@@ -1950,6 +2015,7 @@
     </row>
     <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -1960,7 +2026,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.950000000000001</v>
       </c>
       <c r="E36" s="5">
@@ -1979,6 +2045,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J36" s="5">
@@ -1992,6 +2059,7 @@
     </row>
     <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
@@ -2002,7 +2070,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.950000000000001</v>
       </c>
       <c r="E37" s="5">
@@ -2021,6 +2089,7 @@
         <v>26</v>
       </c>
       <c r="I37" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J37" s="5">
@@ -2034,6 +2103,7 @@
     </row>
     <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="B38" s="11" t="s">
@@ -2044,7 +2114,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15.950000000000001</v>
       </c>
       <c r="E38" s="5">
@@ -2063,6 +2133,7 @@
         <v>27</v>
       </c>
       <c r="I38" s="4">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J38" s="5">

</xml_diff>